<commit_message>
update tc and file jar
</commit_message>
<xml_diff>
--- a/config/testcases/Report_MSP.ChW(Clone).xlsx
+++ b/config/testcases/Report_MSP.ChW(Clone).xlsx
@@ -13,14 +13,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="TUgvnbgiXdEXNj1LeMOx15yT3ChfkyclkMA70TIopbQ="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="i3/pIGfodAxMdeRBFqOixM2LL36Xgo1A2MXSN07Y42o="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="128">
   <si>
     <t>TCID</t>
   </si>
@@ -256,18 +256,6 @@
     <t>$.act[?(@.game_name=="MSP.ChW(Clone)")].turn[0].word[?(@.type=='answer_data')].image[*].file_path</t>
   </si>
   <si>
-    <t>Kiểm tra audio câu trả lời</t>
-  </si>
-  <si>
-    <t>getAudiosSource</t>
-  </si>
-  <si>
-    <t>Managers/SoundManager/FxSource</t>
-  </si>
-  <si>
-    <t>$.act[?(@.game_name=="MSP.ChW(Clone)")].turn[0].word[?(@.type=='answer_data')].audio[*].file_path</t>
-  </si>
-  <si>
     <t>Chờ đáp án xuất hiện</t>
   </si>
   <si>
@@ -352,6 +340,9 @@
     <t>TS5</t>
   </si>
   <si>
+    <t>Kiểm tra audio câu trả lời</t>
+  </si>
+  <si>
     <t>waitForObjectNotPresent</t>
   </si>
   <si>
@@ -359,6 +350,9 @@
   </si>
   <si>
     <t>isElementDisplay</t>
+  </si>
+  <si>
+    <t>$.act[?(@.game_name=="MSP.ChW(Clone)")].turn[0].word[?(@.type=='answer_data')].audio[*].file_path</t>
   </si>
   <si>
     <t>Đợi câu hỏi 2 xuất hiện</t>
@@ -388,19 +382,16 @@
     <t>$.act[?(@.game_name=="MSP.ChW(Clone)")].turn[1].word[?(@.type=='answer_data')].image[*].file_path</t>
   </si>
   <si>
-    <t>$.act[?(@.game_name=="MSP.ChW(Clone)")].turn[1].word[?(@.type=='answer_data')].audio[*].file_path</t>
-  </si>
-  <si>
     <t>$.act[?(@.game_name=="MSP.ChW(Clone)")].turn[1].word[?(@.type=='answer')].text_boolean_</t>
   </si>
   <si>
     <t>$.act[?(@.game_name=="MSP.ChW(Clone)")].turn[1].word[?(@.type=='answer')].audio[*].file_path</t>
   </si>
   <si>
-    <t>TS6</t>
+    <t>$.act[?(@.game_name=="MSP.ChW(Clone)")].turn[1].right_answer.text</t>
   </si>
   <si>
-    <t>$.act[?(@.game_name=="MSP.ChW(Clone)")].turn[1].right_answer.text</t>
+    <t>$.act[?(@.game_name=="MSP.ChW(Clone)")].turn[1].word[?(@.type=='answer_data')].audio[*].file_path</t>
   </si>
   <si>
     <t>Kiểm tra kết thúc game</t>
@@ -1892,62 +1883,60 @@
       <c r="M8" s="34"/>
       <c r="N8" s="34"/>
     </row>
-    <row r="9" ht="38.25" customHeight="1">
-      <c r="A9" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="26" t="s">
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="42" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="31" t="s">
+      <c r="D9" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="43"/>
+      <c r="G9" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="J9" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="K9" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
+      <c r="H9" s="43"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+    </row>
+    <row r="10" ht="25.5" customHeight="1">
       <c r="A10" s="42" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>83</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="43"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="43"/>
       <c r="G10" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="43"/>
-      <c r="I10" s="45"/>
+      <c r="H10" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="36" t="s">
+        <v>82</v>
+      </c>
       <c r="J10" s="43"/>
-      <c r="K10" s="46"/>
+      <c r="K10" s="30" t="s">
+        <v>83</v>
+      </c>
       <c r="L10" s="43"/>
       <c r="M10" s="43"/>
       <c r="N10" s="43"/>
@@ -1957,139 +1946,139 @@
         <v>20</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C11" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="48"/>
+      <c r="D11" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>86</v>
+      </c>
       <c r="F11" s="43"/>
       <c r="G11" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I11" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="J11" s="43"/>
-      <c r="K11" s="30" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="K11" s="38" t="s">
+        <v>72</v>
       </c>
       <c r="L11" s="43"/>
       <c r="M11" s="43"/>
       <c r="N11" s="43"/>
     </row>
-    <row r="12" ht="25.5" customHeight="1">
+    <row r="12" ht="37.5" customHeight="1">
       <c r="A12" s="42" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="49" t="s">
         <v>90</v>
       </c>
+      <c r="D12" s="50"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="43"/>
       <c r="G12" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H12" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="K12" s="38" t="s">
-        <v>72</v>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30" t="s">
+        <v>83</v>
       </c>
       <c r="L12" s="43"/>
       <c r="M12" s="43"/>
       <c r="N12" s="43"/>
     </row>
-    <row r="13" ht="37.5" customHeight="1">
+    <row r="13" ht="25.5" customHeight="1">
       <c r="A13" s="42" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="C13" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="48"/>
       <c r="F13" s="43"/>
       <c r="G13" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I13" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" s="38" t="s">
+        <v>72</v>
       </c>
       <c r="L13" s="43"/>
       <c r="M13" s="43"/>
       <c r="N13" s="43"/>
     </row>
-    <row r="14" ht="25.5" customHeight="1">
-      <c r="A14" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="42" t="s">
+    <row r="14" ht="48.75" customHeight="1">
+      <c r="A14" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="E14" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="49" t="s">
+      <c r="F14" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44" t="s">
+      <c r="G14" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="I14" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="J14" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="K14" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
     </row>
     <row r="15" ht="48.75" customHeight="1">
       <c r="A15" s="26" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>99</v>
@@ -2100,9 +2089,7 @@
       <c r="E15" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="F15" s="30" t="s">
-        <v>102</v>
-      </c>
+      <c r="F15" s="30"/>
       <c r="G15" s="31" t="s">
         <v>15</v>
       </c>
@@ -2114,40 +2101,40 @@
       <c r="M15" s="33"/>
       <c r="N15" s="33"/>
     </row>
-    <row r="16" ht="48.75" customHeight="1">
-      <c r="A16" s="26" t="s">
+    <row r="16" ht="30.0" customHeight="1">
+      <c r="A16" s="42" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="E16" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="F16" s="43"/>
+      <c r="G16" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="43"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+    </row>
+    <row r="17" ht="60.0" customHeight="1">
+      <c r="A17" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="26" t="s">
         <v>105</v>
-      </c>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="34"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-    </row>
-    <row r="17" ht="30.0" customHeight="1">
-      <c r="A17" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>58</v>
       </c>
       <c r="C17" s="47" t="s">
         <v>106</v>
@@ -2162,116 +2149,118 @@
       <c r="G17" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="43"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="46"/>
+      <c r="H17" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="I17" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="K17" s="38" t="s">
+        <v>72</v>
+      </c>
       <c r="L17" s="37"/>
       <c r="M17" s="37"/>
       <c r="N17" s="37"/>
     </row>
-    <row r="18" ht="60.0" customHeight="1">
-      <c r="A18" s="42" t="s">
-        <v>24</v>
+    <row r="18" ht="51.75" customHeight="1">
+      <c r="A18" s="26" t="s">
+        <v>26</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>78</v>
+        <v>50</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>111</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="I18" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="K18" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-    </row>
-    <row r="19" ht="51.75" customHeight="1">
-      <c r="A19" s="26" t="s">
+      <c r="H18" s="28"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+    </row>
+    <row r="19" ht="52.5" customHeight="1">
+      <c r="A19" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>50</v>
+      <c r="B19" s="42" t="s">
+        <v>54</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="E19" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="28"/>
       <c r="I19" s="32"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-    </row>
-    <row r="20" ht="52.5" customHeight="1">
-      <c r="A20" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="42" t="s">
-        <v>54</v>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+    </row>
+    <row r="20" ht="55.5" customHeight="1">
+      <c r="A20" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="51"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="37"/>
+      <c r="K20" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="G20" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
     </row>
     <row r="21" ht="55.5" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>117</v>
@@ -2282,197 +2271,201 @@
       <c r="G21" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="J21" s="37"/>
-      <c r="K21" s="30" t="s">
+      <c r="H21" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="55" t="s">
         <v>118</v>
+      </c>
+      <c r="K21" s="56" t="s">
+        <v>72</v>
       </c>
       <c r="L21" s="53"/>
       <c r="M21" s="53"/>
       <c r="N21" s="53"/>
     </row>
-    <row r="22" ht="55.5" customHeight="1">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="D22" s="51"/>
-      <c r="E22" s="52"/>
+        <v>73</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>74</v>
+      </c>
       <c r="F22" s="34"/>
       <c r="G22" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="I22" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="J22" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="K22" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
-      <c r="N22" s="53"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
+      <c r="H22" s="34"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+    </row>
+    <row r="23" ht="38.25" customHeight="1">
       <c r="A23" s="26" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>74</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
       <c r="F23" s="34"/>
       <c r="G23" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="34"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="40"/>
+      <c r="H23" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="K23" s="38" t="s">
+        <v>72</v>
+      </c>
       <c r="L23" s="34"/>
       <c r="M23" s="34"/>
       <c r="N23" s="34"/>
     </row>
     <row r="24" ht="38.25" customHeight="1">
       <c r="A24" s="26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
+        <v>78</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>79</v>
+      </c>
       <c r="F24" s="34"/>
       <c r="G24" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="I24" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="J24" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="K24" s="38" t="s">
-        <v>72</v>
-      </c>
+      <c r="H24" s="28"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="57"/>
       <c r="L24" s="34"/>
       <c r="M24" s="34"/>
       <c r="N24" s="34"/>
     </row>
-    <row r="25" ht="38.25" customHeight="1">
-      <c r="A25" s="26" t="s">
+    <row r="25" ht="35.25" customHeight="1">
+      <c r="A25" s="42" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="43"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="I25" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="J25" s="30" t="s">
-        <v>122</v>
-      </c>
+      <c r="H25" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="I25" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="J25" s="43"/>
       <c r="K25" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-    </row>
-    <row r="26" ht="38.25" customHeight="1">
-      <c r="A26" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+    </row>
+    <row r="26" ht="25.5" customHeight="1">
+      <c r="A26" s="42" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="43"/>
+      <c r="G26" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="28"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
+      <c r="H26" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="J26" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="K26" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
     </row>
     <row r="27" ht="35.25" customHeight="1">
       <c r="A27" s="42" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="C27" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="43"/>
+        <v>90</v>
+      </c>
+      <c r="D27" s="50"/>
       <c r="E27" s="48"/>
       <c r="F27" s="43"/>
       <c r="G27" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H27" s="35" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I27" s="36" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="J27" s="43"/>
       <c r="K27" s="30" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L27" s="37"/>
       <c r="M27" s="37"/>
@@ -2483,29 +2476,29 @@
         <v>32</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C28" s="47" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E28" s="49" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F28" s="43"/>
       <c r="G28" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H28" s="35" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I28" s="36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J28" s="30" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="K28" s="38" t="s">
         <v>72</v>
@@ -2514,249 +2507,183 @@
       <c r="M28" s="43"/>
       <c r="N28" s="43"/>
     </row>
-    <row r="29" ht="35.25" customHeight="1">
-      <c r="A29" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="26" t="s">
+    <row r="29" ht="40.5" customHeight="1">
+      <c r="A29" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G29" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="63"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="63"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+    </row>
+    <row r="30" ht="40.5" customHeight="1">
+      <c r="A30" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="46"/>
+      <c r="G30" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="63"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="63"/>
+      <c r="L30" s="63"/>
+      <c r="M30" s="63"/>
+      <c r="N30" s="63"/>
+    </row>
+    <row r="31" ht="30.0" customHeight="1">
+      <c r="A31" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="43"/>
+      <c r="G31" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="43"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="37"/>
+    </row>
+    <row r="32" ht="60.0" customHeight="1">
+      <c r="A32" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="44" t="s">
+      <c r="I32" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="J32" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="K32" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="F33" s="34"/>
+      <c r="G33" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H29" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="I29" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="J29" s="43"/>
-      <c r="K29" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-    </row>
-    <row r="30" ht="25.5" customHeight="1">
-      <c r="A30" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="C30" s="47" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="E30" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" s="43"/>
-      <c r="G30" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="I30" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="J30" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="K30" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43"/>
-    </row>
-    <row r="31" ht="40.5" customHeight="1">
-      <c r="A31" s="58" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="59" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="E31" s="61" t="s">
-        <v>101</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="G31" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="63"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="63"/>
-      <c r="K31" s="63"/>
-      <c r="L31" s="63"/>
-      <c r="M31" s="63"/>
-      <c r="N31" s="63"/>
-    </row>
-    <row r="32" ht="40.5" customHeight="1">
-      <c r="A32" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="F32" s="46"/>
-      <c r="G32" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="63"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="63"/>
-    </row>
-    <row r="33" ht="30.0" customHeight="1">
-      <c r="A33" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="F33" s="43"/>
-      <c r="G33" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="43"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="37"/>
-    </row>
-    <row r="34" ht="60.0" customHeight="1">
-      <c r="A34" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="E34" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H34" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="I34" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="J34" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="K34" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="L34" s="37"/>
-      <c r="M34" s="37"/>
-      <c r="N34" s="37"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="D35" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="F35" s="34"/>
-      <c r="G35" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="34"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="40"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="33"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L1:L35 M1:N1">
+  <conditionalFormatting sqref="L1:L33 M1:N1">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L35 M1:N1">
+  <conditionalFormatting sqref="L1:L33 M1:N1">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L35 M1:N1">
+  <conditionalFormatting sqref="L1:L33 M1:N1">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"SKIP"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H6 H8 H21:H22 H26">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H6 H8 H23">
       <formula1>Keywords!$A$2:$A168</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H31:H33">
-      <formula1>Keywords!$A$2:$A186</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H12 H14:H15 H25 H27">
+      <formula1>Keywords!$A$2:$A167</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H18 H27 H29">
-      <formula1>Keywords!$A$2:$A171</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H16">
+      <formula1>Keywords!$A$2:$A169</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A1:A35">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A1:A33">
       <formula1>TestCase!$A:$A</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2">
@@ -2765,35 +2692,35 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H7">
       <formula1>Keywords!$A$2:$A166</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H24">
-      <formula1>Keywords!$A$2:$A185</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H22">
+      <formula1>Keywords!$A$2:$A183</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H10:H12 H14 D2:D35">
-      <formula1>Keywords!$A$2:$A35</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9:H11 H13 D2:D33">
+      <formula1>Keywords!$A$2:$A33</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H29:H31">
+      <formula1>Keywords!$A$2:$A186</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H33">
+      <formula1>Keywords!$A$2:$A180</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H19 H24">
+      <formula1>Keywords!$A$2:$A183</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G33">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H5">
+      <formula1>Keywords!$A$2:$A165</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H3:H4 H20:H21">
+      <formula1>Keywords!$A$2:$A166</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H18 H26 H28 H32">
+      <formula1>Keywords!$A$2:$A176</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H17">
-      <formula1>Keywords!$A$2:$A169</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H9 H28 H30 H34">
-      <formula1>Keywords!$A$2:$A165</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H19 H25">
-      <formula1>Keywords!$A$2:$A176</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G35">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H35">
-      <formula1>Keywords!$A$2:$A180</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H5 H23">
-      <formula1>Keywords!$A$2:$A165</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H3:H4 H20">
-      <formula1>Keywords!$A$2:$A166</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H13 H15:H16">
-      <formula1>Keywords!$A$2:$A167</formula1>
+      <formula1>Keywords!$A$2:$A171</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>
@@ -2823,10 +2750,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="65" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C1" s="65" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>

</xml_diff>